<commit_message>
hace dos semanas lo subi
</commit_message>
<xml_diff>
--- a/Requisitos/RequisitosProestheticVersionBeta.xlsx.xlsx.xlsx
+++ b/Requisitos/RequisitosProestheticVersionBeta.xlsx.xlsx.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17668"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1725,14 +1725,17 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1770,7 +1773,10 @@
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1792,6 +1798,9 @@
     <xf numFmtId="0" fontId="3" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1800,15 +1809,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2156,7 +2156,7 @@
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2181,7 +2181,7 @@
       <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="79" t="s">
+      <c r="C2" s="94" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="17"/>
@@ -2193,7 +2193,7 @@
       <c r="B3" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="104"/>
+      <c r="C3" s="95"/>
       <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2203,7 +2203,7 @@
       <c r="B4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="104"/>
+      <c r="C4" s="95"/>
       <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2213,7 +2213,7 @@
       <c r="B5" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="104"/>
+      <c r="C5" s="95"/>
       <c r="D5" s="23"/>
     </row>
     <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2223,7 +2223,7 @@
       <c r="B6" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="104"/>
+      <c r="C6" s="95"/>
       <c r="D6" s="17"/>
     </row>
     <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2233,7 +2233,7 @@
       <c r="B7" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="104"/>
+      <c r="C7" s="95"/>
       <c r="D7" s="17"/>
     </row>
     <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2243,7 +2243,7 @@
       <c r="B8" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="104"/>
+      <c r="C8" s="95"/>
       <c r="D8" s="17"/>
     </row>
     <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2253,7 +2253,7 @@
       <c r="B9" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="104"/>
+      <c r="C9" s="95"/>
       <c r="D9" s="17"/>
     </row>
     <row r="10" spans="1:4" s="68" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -2263,7 +2263,7 @@
       <c r="B10" s="25" t="s">
         <v>419</v>
       </c>
-      <c r="C10" s="104"/>
+      <c r="C10" s="95"/>
       <c r="D10" s="23"/>
     </row>
     <row r="11" spans="1:4" s="68" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -2273,7 +2273,7 @@
       <c r="B11" s="25" t="s">
         <v>420</v>
       </c>
-      <c r="C11" s="104"/>
+      <c r="C11" s="95"/>
       <c r="D11" s="23"/>
     </row>
     <row r="12" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2283,7 +2283,7 @@
       <c r="B12" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="76" t="s">
+      <c r="C12" s="78" t="s">
         <v>62</v>
       </c>
       <c r="D12" s="17"/>
@@ -2295,7 +2295,7 @@
       <c r="B13" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="77"/>
+      <c r="C13" s="79"/>
       <c r="D13" s="17"/>
     </row>
     <row r="14" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2305,7 +2305,7 @@
       <c r="B14" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="77"/>
+      <c r="C14" s="79"/>
       <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2315,7 +2315,7 @@
       <c r="B15" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="77"/>
+      <c r="C15" s="79"/>
       <c r="D15" s="17"/>
     </row>
     <row r="16" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2325,7 +2325,7 @@
       <c r="B16" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="78"/>
+      <c r="C16" s="80"/>
       <c r="D16" s="17"/>
     </row>
     <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -2335,7 +2335,7 @@
       <c r="B17" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="85" t="s">
+      <c r="C17" s="86" t="s">
         <v>87</v>
       </c>
       <c r="D17" s="23" t="s">
@@ -2349,7 +2349,7 @@
       <c r="B18" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="C18" s="86"/>
+      <c r="C18" s="87"/>
       <c r="D18" s="17"/>
     </row>
     <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -2359,7 +2359,7 @@
       <c r="B19" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="86"/>
+      <c r="C19" s="87"/>
       <c r="D19" s="17"/>
     </row>
     <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -2369,7 +2369,7 @@
       <c r="B20" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="C20" s="86"/>
+      <c r="C20" s="87"/>
       <c r="D20" s="17"/>
     </row>
     <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -2379,7 +2379,7 @@
       <c r="B21" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="86"/>
+      <c r="C21" s="87"/>
       <c r="D21" s="17"/>
     </row>
     <row r="22" spans="1:5" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -2389,7 +2389,7 @@
       <c r="B22" s="72" t="s">
         <v>418</v>
       </c>
-      <c r="C22" s="86"/>
+      <c r="C22" s="87"/>
       <c r="D22" s="23"/>
     </row>
     <row r="23" spans="1:5" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -2399,7 +2399,7 @@
       <c r="B23" s="36" t="s">
         <v>378</v>
       </c>
-      <c r="C23" s="87"/>
+      <c r="C23" s="88"/>
       <c r="D23" s="23"/>
     </row>
     <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -2409,7 +2409,7 @@
       <c r="B24" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="90" t="s">
+      <c r="C24" s="91" t="s">
         <v>113</v>
       </c>
       <c r="D24" s="17"/>
@@ -2421,7 +2421,7 @@
       <c r="B25" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="C25" s="77"/>
+      <c r="C25" s="79"/>
       <c r="D25" s="17"/>
       <c r="E25" s="23"/>
     </row>
@@ -2432,7 +2432,7 @@
       <c r="B26" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="C26" s="77"/>
+      <c r="C26" s="79"/>
       <c r="D26" s="17"/>
     </row>
     <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -2442,7 +2442,7 @@
       <c r="B27" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="C27" s="78"/>
+      <c r="C27" s="80"/>
       <c r="D27" s="17"/>
     </row>
     <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -2452,7 +2452,7 @@
       <c r="B28" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="C28" s="80" t="s">
+      <c r="C28" s="81" t="s">
         <v>403</v>
       </c>
       <c r="D28" s="17"/>
@@ -2464,7 +2464,7 @@
       <c r="B29" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="C29" s="81"/>
+      <c r="C29" s="82"/>
       <c r="D29" s="17"/>
     </row>
     <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -2474,7 +2474,7 @@
       <c r="B30" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="C30" s="81"/>
+      <c r="C30" s="82"/>
       <c r="D30" s="17"/>
     </row>
     <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -2484,7 +2484,7 @@
       <c r="B31" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="C31" s="81"/>
+      <c r="C31" s="82"/>
       <c r="D31" s="23"/>
     </row>
     <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -2494,7 +2494,7 @@
       <c r="B32" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="C32" s="81"/>
+      <c r="C32" s="82"/>
       <c r="D32" s="17"/>
     </row>
     <row r="33" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2504,7 +2504,7 @@
       <c r="B33" s="45" t="s">
         <v>150</v>
       </c>
-      <c r="C33" s="81"/>
+      <c r="C33" s="82"/>
       <c r="D33" s="17"/>
     </row>
     <row r="34" spans="1:4" s="68" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -2514,7 +2514,7 @@
       <c r="B34" s="45" t="s">
         <v>406</v>
       </c>
-      <c r="C34" s="81"/>
+      <c r="C34" s="82"/>
       <c r="D34" s="23"/>
     </row>
     <row r="35" spans="1:4" s="68" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -2524,7 +2524,7 @@
       <c r="B35" s="45" t="s">
         <v>405</v>
       </c>
-      <c r="C35" s="81"/>
+      <c r="C35" s="82"/>
       <c r="D35" s="23"/>
     </row>
     <row r="36" spans="1:4" s="68" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -2534,7 +2534,7 @@
       <c r="B36" s="45" t="s">
         <v>409</v>
       </c>
-      <c r="C36" s="82"/>
+      <c r="C36" s="83"/>
       <c r="D36" s="23"/>
     </row>
     <row r="37" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2544,7 +2544,7 @@
       <c r="B37" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="C37" s="92" t="s">
+      <c r="C37" s="93" t="s">
         <v>167</v>
       </c>
       <c r="D37" s="17"/>
@@ -2556,7 +2556,7 @@
       <c r="B38" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="C38" s="77"/>
+      <c r="C38" s="79"/>
       <c r="D38" s="17"/>
     </row>
     <row r="39" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2566,7 +2566,7 @@
       <c r="B39" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="C39" s="77"/>
+      <c r="C39" s="79"/>
       <c r="D39" s="17"/>
     </row>
     <row r="40" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2576,7 +2576,7 @@
       <c r="B40" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="C40" s="77"/>
+      <c r="C40" s="79"/>
       <c r="D40" s="17"/>
     </row>
     <row r="41" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2586,7 +2586,7 @@
       <c r="B41" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="C41" s="77"/>
+      <c r="C41" s="79"/>
       <c r="D41" s="17"/>
     </row>
     <row r="42" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2596,7 +2596,7 @@
       <c r="B42" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="C42" s="78"/>
+      <c r="C42" s="80"/>
       <c r="D42" s="17"/>
     </row>
     <row r="43" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2606,7 +2606,7 @@
       <c r="B43" s="49" t="s">
         <v>194</v>
       </c>
-      <c r="C43" s="88" t="s">
+      <c r="C43" s="89" t="s">
         <v>195</v>
       </c>
       <c r="D43" s="17"/>
@@ -2618,7 +2618,7 @@
       <c r="B44" s="36" t="s">
         <v>199</v>
       </c>
-      <c r="C44" s="77"/>
+      <c r="C44" s="79"/>
       <c r="D44" s="17"/>
     </row>
     <row r="45" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2628,7 +2628,7 @@
       <c r="B45" s="49" t="s">
         <v>201</v>
       </c>
-      <c r="C45" s="77"/>
+      <c r="C45" s="79"/>
       <c r="D45" s="17"/>
     </row>
     <row r="46" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2638,7 +2638,7 @@
       <c r="B46" s="36" t="s">
         <v>203</v>
       </c>
-      <c r="C46" s="77"/>
+      <c r="C46" s="79"/>
       <c r="D46" s="17"/>
     </row>
     <row r="47" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2648,7 +2648,7 @@
       <c r="B47" s="49" t="s">
         <v>207</v>
       </c>
-      <c r="C47" s="77"/>
+      <c r="C47" s="79"/>
       <c r="D47" s="17"/>
     </row>
     <row r="48" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2658,7 +2658,7 @@
       <c r="B48" s="36" t="s">
         <v>209</v>
       </c>
-      <c r="C48" s="77"/>
+      <c r="C48" s="79"/>
       <c r="D48" s="17"/>
     </row>
     <row r="49" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2668,7 +2668,7 @@
       <c r="B49" s="49" t="s">
         <v>211</v>
       </c>
-      <c r="C49" s="78"/>
+      <c r="C49" s="80"/>
       <c r="D49" s="17"/>
     </row>
     <row r="50" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2678,7 +2678,7 @@
       <c r="B50" s="30" t="s">
         <v>217</v>
       </c>
-      <c r="C50" s="91" t="s">
+      <c r="C50" s="92" t="s">
         <v>218</v>
       </c>
       <c r="D50" s="17"/>
@@ -2690,7 +2690,7 @@
       <c r="B51" s="54" t="s">
         <v>224</v>
       </c>
-      <c r="C51" s="77"/>
+      <c r="C51" s="79"/>
       <c r="D51" s="17"/>
     </row>
     <row r="52" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2700,7 +2700,7 @@
       <c r="B52" s="54" t="s">
         <v>226</v>
       </c>
-      <c r="C52" s="77"/>
+      <c r="C52" s="79"/>
       <c r="D52" s="17"/>
     </row>
     <row r="53" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2710,7 +2710,7 @@
       <c r="B53" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="C53" s="78"/>
+      <c r="C53" s="80"/>
       <c r="D53" s="17"/>
     </row>
     <row r="54" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -2720,7 +2720,7 @@
       <c r="B54" s="55" t="s">
         <v>232</v>
       </c>
-      <c r="C54" s="89" t="s">
+      <c r="C54" s="90" t="s">
         <v>233</v>
       </c>
     </row>
@@ -2731,7 +2731,7 @@
       <c r="B55" s="57" t="s">
         <v>242</v>
       </c>
-      <c r="C55" s="77"/>
+      <c r="C55" s="79"/>
     </row>
     <row r="56" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="55" t="s">
@@ -2740,7 +2740,7 @@
       <c r="B56" s="55" t="s">
         <v>244</v>
       </c>
-      <c r="C56" s="77"/>
+      <c r="C56" s="79"/>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="69" t="s">
@@ -2749,7 +2749,7 @@
       <c r="B57" s="69" t="s">
         <v>373</v>
       </c>
-      <c r="C57" s="83" t="s">
+      <c r="C57" s="84" t="s">
         <v>389</v>
       </c>
     </row>
@@ -2760,7 +2760,7 @@
       <c r="B58" s="70" t="s">
         <v>374</v>
       </c>
-      <c r="C58" s="84"/>
+      <c r="C58" s="85"/>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="69" t="s">
@@ -2769,7 +2769,7 @@
       <c r="B59" s="69" t="s">
         <v>375</v>
       </c>
-      <c r="C59" s="84"/>
+      <c r="C59" s="85"/>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="73" t="s">
@@ -2778,7 +2778,7 @@
       <c r="B60" s="73" t="s">
         <v>426</v>
       </c>
-      <c r="C60" s="105" t="s">
+      <c r="C60" s="76" t="s">
         <v>391</v>
       </c>
     </row>
@@ -2789,7 +2789,7 @@
       <c r="B61" t="s">
         <v>395</v>
       </c>
-      <c r="C61" s="106"/>
+      <c r="C61" s="77"/>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="73" t="s">
@@ -2798,10 +2798,11 @@
       <c r="B62" t="s">
         <v>396</v>
       </c>
-      <c r="C62" s="106"/>
+      <c r="C62" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C2:C11"/>
     <mergeCell ref="C60:C62"/>
     <mergeCell ref="C12:C16"/>
     <mergeCell ref="C28:C36"/>
@@ -2812,7 +2813,6 @@
     <mergeCell ref="C24:C27"/>
     <mergeCell ref="C50:C53"/>
     <mergeCell ref="C37:C42"/>
-    <mergeCell ref="C2:C11"/>
   </mergeCells>
   <conditionalFormatting sqref="A43:C43 A45:B45 A47:B47 A49:B49">
     <cfRule type="notContainsBlanks" dxfId="1" priority="1">
@@ -2858,10 +2858,10 @@
       <c r="B2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="98" t="s">
+      <c r="C2" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="94">
+      <c r="D2" s="96">
         <v>1</v>
       </c>
       <c r="E2" s="7"/>
@@ -2873,8 +2873,8 @@
       <c r="B3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="95"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="97"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2884,8 +2884,8 @@
       <c r="B4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="95"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="97"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2895,8 +2895,8 @@
       <c r="B5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="77"/>
-      <c r="D5" s="95"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="97"/>
       <c r="E5" s="16" t="s">
         <v>23</v>
       </c>
@@ -2908,8 +2908,8 @@
       <c r="B6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="77"/>
-      <c r="D6" s="95"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="97"/>
       <c r="E6" s="20"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2919,8 +2919,8 @@
       <c r="B7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="78"/>
-      <c r="D7" s="95"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="97"/>
       <c r="E7" s="20"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2930,10 +2930,10 @@
       <c r="B8" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="94">
+      <c r="D8" s="96">
         <v>2</v>
       </c>
       <c r="E8" s="7"/>
@@ -2945,8 +2945,8 @@
       <c r="B9" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="77"/>
-      <c r="D9" s="95"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="97"/>
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2956,8 +2956,8 @@
       <c r="B10" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="95"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="97"/>
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2967,8 +2967,8 @@
       <c r="B11" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="77"/>
-      <c r="D11" s="95"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="97"/>
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2978,8 +2978,8 @@
       <c r="B12" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="77"/>
-      <c r="D12" s="95"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="97"/>
       <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2989,8 +2989,8 @@
       <c r="B13" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="78"/>
-      <c r="D13" s="95"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="97"/>
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3000,10 +3000,10 @@
       <c r="B14" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="99" t="s">
+      <c r="C14" s="101" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="94">
+      <c r="D14" s="96">
         <v>3</v>
       </c>
       <c r="E14" s="7"/>
@@ -3015,8 +3015,8 @@
       <c r="B15" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="77"/>
-      <c r="D15" s="95"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="97"/>
       <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3026,8 +3026,8 @@
       <c r="B16" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="77"/>
-      <c r="D16" s="95"/>
+      <c r="C16" s="79"/>
+      <c r="D16" s="97"/>
       <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3037,8 +3037,8 @@
       <c r="B17" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="77"/>
-      <c r="D17" s="95"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="97"/>
       <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3048,8 +3048,8 @@
       <c r="B18" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="77"/>
-      <c r="D18" s="95"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="97"/>
       <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3059,8 +3059,8 @@
       <c r="B19" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="C19" s="77"/>
-      <c r="D19" s="95"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="97"/>
       <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3070,8 +3070,8 @@
       <c r="B20" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="C20" s="77"/>
-      <c r="D20" s="95"/>
+      <c r="C20" s="79"/>
+      <c r="D20" s="97"/>
       <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3081,8 +3081,8 @@
       <c r="B21" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="77"/>
-      <c r="D21" s="95"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="97"/>
       <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3092,10 +3092,10 @@
       <c r="B22" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="C22" s="97" t="s">
+      <c r="C22" s="99" t="s">
         <v>114</v>
       </c>
-      <c r="D22" s="94">
+      <c r="D22" s="96">
         <v>6</v>
       </c>
       <c r="E22" s="7"/>
@@ -3107,8 +3107,8 @@
       <c r="B23" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="C23" s="77"/>
-      <c r="D23" s="95"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="97"/>
       <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3118,8 +3118,8 @@
       <c r="B24" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="C24" s="77"/>
-      <c r="D24" s="95"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="97"/>
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3129,8 +3129,8 @@
       <c r="B25" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="C25" s="77"/>
-      <c r="D25" s="95"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="97"/>
       <c r="E25" s="16" t="s">
         <v>128</v>
       </c>
@@ -3142,8 +3142,8 @@
       <c r="B26" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="95"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="97"/>
       <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3153,8 +3153,8 @@
       <c r="B27" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="C27" s="77"/>
-      <c r="D27" s="95"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="97"/>
       <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3164,8 +3164,8 @@
       <c r="B28" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="C28" s="77"/>
-      <c r="D28" s="95"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="97"/>
       <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3175,10 +3175,10 @@
       <c r="B29" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="C29" s="85" t="s">
+      <c r="C29" s="86" t="s">
         <v>139</v>
       </c>
-      <c r="D29" s="94">
+      <c r="D29" s="96">
         <v>4</v>
       </c>
       <c r="E29" s="7"/>
@@ -3190,8 +3190,8 @@
       <c r="B30" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="C30" s="77"/>
-      <c r="D30" s="95"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="97"/>
       <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3201,8 +3201,8 @@
       <c r="B31" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="C31" s="77"/>
-      <c r="D31" s="95"/>
+      <c r="C31" s="79"/>
+      <c r="D31" s="97"/>
       <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3212,8 +3212,8 @@
       <c r="B32" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="C32" s="77"/>
-      <c r="D32" s="95"/>
+      <c r="C32" s="79"/>
+      <c r="D32" s="97"/>
       <c r="E32" s="16" t="s">
         <v>128</v>
       </c>
@@ -3225,8 +3225,8 @@
       <c r="B33" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="C33" s="77"/>
-      <c r="D33" s="95"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="97"/>
       <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3236,8 +3236,8 @@
       <c r="B34" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="C34" s="77"/>
-      <c r="D34" s="95"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="97"/>
       <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3247,8 +3247,8 @@
       <c r="B35" s="44" t="s">
         <v>160</v>
       </c>
-      <c r="C35" s="77"/>
-      <c r="D35" s="95"/>
+      <c r="C35" s="79"/>
+      <c r="D35" s="97"/>
       <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3258,8 +3258,8 @@
       <c r="B36" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="C36" s="77"/>
-      <c r="D36" s="94">
+      <c r="C36" s="79"/>
+      <c r="D36" s="96">
         <v>5</v>
       </c>
       <c r="E36" s="7"/>
@@ -3271,10 +3271,10 @@
       <c r="B37" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="C37" s="93" t="s">
+      <c r="C37" s="103" t="s">
         <v>168</v>
       </c>
-      <c r="D37" s="95"/>
+      <c r="D37" s="97"/>
       <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3284,8 +3284,8 @@
       <c r="B38" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C38" s="77"/>
-      <c r="D38" s="95"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="97"/>
       <c r="E38" s="7"/>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3295,8 +3295,8 @@
       <c r="B39" s="47" t="s">
         <v>183</v>
       </c>
-      <c r="C39" s="77"/>
-      <c r="D39" s="95"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="97"/>
       <c r="E39" s="16" t="s">
         <v>184</v>
       </c>
@@ -3308,8 +3308,8 @@
       <c r="B40" s="48" t="s">
         <v>186</v>
       </c>
-      <c r="C40" s="77"/>
-      <c r="D40" s="95"/>
+      <c r="C40" s="79"/>
+      <c r="D40" s="97"/>
       <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3319,8 +3319,8 @@
       <c r="B41" s="47" t="s">
         <v>188</v>
       </c>
-      <c r="C41" s="77"/>
-      <c r="D41" s="95"/>
+      <c r="C41" s="79"/>
+      <c r="D41" s="97"/>
       <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3330,8 +3330,8 @@
       <c r="B42" s="34" t="s">
         <v>190</v>
       </c>
-      <c r="C42" s="77"/>
-      <c r="D42" s="95"/>
+      <c r="C42" s="79"/>
+      <c r="D42" s="97"/>
       <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3341,10 +3341,10 @@
       <c r="B43" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="C43" s="92" t="s">
+      <c r="C43" s="93" t="s">
         <v>193</v>
       </c>
-      <c r="D43" s="94">
+      <c r="D43" s="96">
         <v>7</v>
       </c>
       <c r="E43" s="7"/>
@@ -3356,8 +3356,8 @@
       <c r="B44" s="50" t="s">
         <v>197</v>
       </c>
-      <c r="C44" s="77"/>
-      <c r="D44" s="95"/>
+      <c r="C44" s="79"/>
+      <c r="D44" s="97"/>
       <c r="E44" s="7"/>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3367,8 +3367,8 @@
       <c r="B45" s="51" t="s">
         <v>205</v>
       </c>
-      <c r="C45" s="77"/>
-      <c r="D45" s="95"/>
+      <c r="C45" s="79"/>
+      <c r="D45" s="97"/>
       <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3378,8 +3378,8 @@
       <c r="B46" s="50" t="s">
         <v>213</v>
       </c>
-      <c r="C46" s="77"/>
-      <c r="D46" s="95"/>
+      <c r="C46" s="79"/>
+      <c r="D46" s="97"/>
       <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3389,8 +3389,8 @@
       <c r="B47" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="C47" s="77"/>
-      <c r="D47" s="95"/>
+      <c r="C47" s="79"/>
+      <c r="D47" s="97"/>
       <c r="E47" s="7"/>
     </row>
     <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3400,8 +3400,8 @@
       <c r="B48" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="C48" s="77"/>
-      <c r="D48" s="95"/>
+      <c r="C48" s="79"/>
+      <c r="D48" s="97"/>
       <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3411,10 +3411,10 @@
       <c r="B49" s="53" t="s">
         <v>221</v>
       </c>
-      <c r="C49" s="100" t="s">
+      <c r="C49" s="102" t="s">
         <v>223</v>
       </c>
-      <c r="D49" s="94">
+      <c r="D49" s="96">
         <v>8</v>
       </c>
       <c r="E49" s="7"/>
@@ -3426,8 +3426,8 @@
       <c r="B50" s="56" t="s">
         <v>231</v>
       </c>
-      <c r="C50" s="77"/>
-      <c r="D50" s="95"/>
+      <c r="C50" s="79"/>
+      <c r="D50" s="97"/>
       <c r="E50" s="7"/>
     </row>
     <row r="51" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3437,8 +3437,8 @@
       <c r="B51" s="53" t="s">
         <v>235</v>
       </c>
-      <c r="C51" s="77"/>
-      <c r="D51" s="95"/>
+      <c r="C51" s="79"/>
+      <c r="D51" s="97"/>
       <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3448,8 +3448,8 @@
       <c r="B52" s="56" t="s">
         <v>203</v>
       </c>
-      <c r="C52" s="77"/>
-      <c r="D52" s="95"/>
+      <c r="C52" s="79"/>
+      <c r="D52" s="97"/>
       <c r="E52" s="7"/>
     </row>
     <row r="53" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3459,8 +3459,8 @@
       <c r="B53" s="53" t="s">
         <v>238</v>
       </c>
-      <c r="C53" s="77"/>
-      <c r="D53" s="95"/>
+      <c r="C53" s="79"/>
+      <c r="D53" s="97"/>
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3470,8 +3470,8 @@
       <c r="B54" s="58" t="s">
         <v>241</v>
       </c>
-      <c r="C54" s="78"/>
-      <c r="D54" s="95"/>
+      <c r="C54" s="80"/>
+      <c r="D54" s="97"/>
       <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3481,10 +3481,10 @@
       <c r="B55" s="59" t="s">
         <v>135</v>
       </c>
-      <c r="C55" s="96" t="s">
+      <c r="C55" s="98" t="s">
         <v>246</v>
       </c>
-      <c r="D55" s="94">
+      <c r="D55" s="96">
         <v>9</v>
       </c>
       <c r="E55" s="7"/>
@@ -3496,8 +3496,8 @@
       <c r="B56" s="60" t="s">
         <v>248</v>
       </c>
-      <c r="C56" s="77"/>
-      <c r="D56" s="95"/>
+      <c r="C56" s="79"/>
+      <c r="D56" s="97"/>
       <c r="E56" s="7"/>
     </row>
     <row r="57" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3507,8 +3507,8 @@
       <c r="B57" s="59" t="s">
         <v>250</v>
       </c>
-      <c r="C57" s="77"/>
-      <c r="D57" s="95"/>
+      <c r="C57" s="79"/>
+      <c r="D57" s="97"/>
       <c r="E57" s="7"/>
     </row>
     <row r="58" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3518,8 +3518,8 @@
       <c r="B58" s="60" t="s">
         <v>252</v>
       </c>
-      <c r="C58" s="77"/>
-      <c r="D58" s="95"/>
+      <c r="C58" s="79"/>
+      <c r="D58" s="97"/>
       <c r="E58" s="16" t="s">
         <v>253</v>
       </c>
@@ -3531,8 +3531,8 @@
       <c r="B59" s="59" t="s">
         <v>146</v>
       </c>
-      <c r="C59" s="77"/>
-      <c r="D59" s="95"/>
+      <c r="C59" s="79"/>
+      <c r="D59" s="97"/>
       <c r="E59" s="7"/>
     </row>
     <row r="60" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3542,8 +3542,8 @@
       <c r="B60" s="60" t="s">
         <v>256</v>
       </c>
-      <c r="C60" s="78"/>
-      <c r="D60" s="95"/>
+      <c r="C60" s="80"/>
+      <c r="D60" s="97"/>
       <c r="E60" s="7"/>
     </row>
     <row r="61" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10128,6 +10128,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D29:D35"/>
+    <mergeCell ref="D2:D7"/>
     <mergeCell ref="D55:D60"/>
     <mergeCell ref="C55:C60"/>
     <mergeCell ref="C22:C28"/>
@@ -10144,8 +10146,6 @@
     <mergeCell ref="C43:C48"/>
     <mergeCell ref="C37:C42"/>
     <mergeCell ref="D49:D54"/>
-    <mergeCell ref="D29:D35"/>
-    <mergeCell ref="D2:D7"/>
   </mergeCells>
   <conditionalFormatting sqref="B49:C49 B51 B53">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
@@ -10199,7 +10199,7 @@
       <c r="B2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="102" t="s">
+      <c r="C2" s="105" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="10"/>
@@ -10219,7 +10219,7 @@
       <c r="B3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="78"/>
+      <c r="C3" s="80"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
@@ -10237,7 +10237,7 @@
       <c r="B4" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="101" t="s">
+      <c r="C4" s="104" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="10"/>
@@ -10257,7 +10257,7 @@
       <c r="B5" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="77"/>
+      <c r="C5" s="79"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
@@ -10275,7 +10275,7 @@
       <c r="B6" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="78"/>
+      <c r="C6" s="80"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
@@ -10293,7 +10293,7 @@
       <c r="B7" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="103" t="s">
+      <c r="C7" s="106" t="s">
         <v>47</v>
       </c>
       <c r="D7" s="10"/>
@@ -10313,7 +10313,7 @@
       <c r="B8" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="77"/>
+      <c r="C8" s="79"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
@@ -10331,7 +10331,7 @@
       <c r="B9" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="77"/>
+      <c r="C9" s="79"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
@@ -10349,7 +10349,7 @@
       <c r="B10" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="78"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>

</xml_diff>